<commit_message>
output for multi file came
</commit_message>
<xml_diff>
--- a/Trail 4/BigDATA/Output/multi_file.xlsx
+++ b/Trail 4/BigDATA/Output/multi_file.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="195">
   <si>
     <t>Requirement Description</t>
   </si>
@@ -528,123 +528,127 @@
     <t>Periodically and actively participate in cyber drills conducted under the aegis of Cert-IN, IDRBT etc.</t>
   </si>
   <si>
+    <t>Authentication Framework</t>
+  </si>
+  <si>
     <t>Other</t>
   </si>
   <si>
-    <t>Authentication Framework</t>
-  </si>
-  <si>
-    <t>Vendor Risk Management</t>
+    <t>Digital Payment Security Controls(Mobile Payment)</t>
+  </si>
+  <si>
+    <t>Governance and Management
+ of Security Risks</t>
+  </si>
+  <si>
+    <t>User/Employee/Management Awareness</t>
   </si>
   <si>
     <t>Business Continuity Plan (BCP)</t>
   </si>
   <si>
-    <t>User Access Control</t>
+    <t>Fraud Risk Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patch &amp; Change Management
+</t>
   </si>
   <si>
     <t>CARD PAYMENTS SECURITY</t>
   </si>
   <si>
-    <t>Authentication Framework for Customers</t>
+    <t>Incident Response</t>
+  </si>
+  <si>
+    <t>Other Security Measures</t>
   </si>
   <si>
     <t>Other Generic Security 
 Controls</t>
   </si>
   <si>
-    <t>Fraud Risk Management</t>
+    <t>Customer Protection, Awareness and Grievance Redressal Mechanism</t>
   </si>
   <si>
     <t>Application Security</t>
   </si>
   <si>
+    <t>Data Security</t>
+  </si>
+  <si>
+    <t>Mobile Payments Application</t>
+  </si>
+  <si>
+    <t>Environmental Controls</t>
+  </si>
+  <si>
+    <t>Customer Education and Awareness</t>
+  </si>
+  <si>
+    <t>Application Programming Interfaces (APIs)</t>
+  </si>
+  <si>
+    <t>Digital Payment Security Controls</t>
+  </si>
+  <si>
+    <t>Secure Configuration</t>
+  </si>
+  <si>
+    <t>User Access Control/Management</t>
+  </si>
+  <si>
+    <t>Application Security Life Cycle (ASLC)</t>
+  </si>
+  <si>
     <t>Incident Response &amp; Management</t>
   </si>
   <si>
-    <t>Employee Awareness / Training</t>
-  </si>
-  <si>
-    <t>Preventing access of 
-unauthorised software</t>
-  </si>
-  <si>
-    <t>Secure Configuration</t>
-  </si>
-  <si>
-    <t>Customer Protection, Awareness and Grievance Redressal Mechanism</t>
-  </si>
-  <si>
-    <t>Governance and Management
- of Security Risks</t>
-  </si>
-  <si>
-    <t>User Access Control/Management</t>
+    <t>Secure mail and messaging systems</t>
+  </si>
+  <si>
+    <t>Network Security</t>
   </si>
   <si>
     <t>Identity and Access 
 Management</t>
   </si>
   <si>
-    <t>Vendor/Outsourcing Risk 
-Management</t>
-  </si>
-  <si>
-    <t>Incident Response</t>
+    <t>Advanced Real-time Threat Defence and Management</t>
+  </si>
+  <si>
+    <t>Audit Logs</t>
+  </si>
+  <si>
+    <t>Expectations from 
+C-SOC</t>
+  </si>
+  <si>
+    <t>Arrangement for continuous 
+surveillance - Setting up of 
+Cyber Security Operation 
+Center (C-SOC)</t>
+  </si>
+  <si>
+    <t>Patch/Vulnerability &amp; Change Management</t>
+  </si>
+  <si>
+    <t>Reconciliation Mechanism</t>
+  </si>
+  <si>
+    <t>Network Management and Security</t>
   </si>
   <si>
     <t>Maintenance, Monitoring, and Analysis of Audit Logs</t>
   </si>
   <si>
-    <t>Data Security</t>
-  </si>
-  <si>
-    <t>Network Management and 
-Security</t>
-  </si>
-  <si>
-    <t>Removable Media</t>
-  </si>
-  <si>
-    <t>Vulnerability assessment, Penetration Test and Red Team
-Exercises</t>
-  </si>
-  <si>
-    <t>Risk based transaction 
-monitoring</t>
-  </si>
-  <si>
-    <t>Data Leak Prevention Strategy</t>
-  </si>
-  <si>
-    <t>User/Employee/Management Awareness</t>
-  </si>
-  <si>
-    <t>Other Security Measures</t>
-  </si>
-  <si>
-    <t>Security Testing</t>
-  </si>
-  <si>
-    <t>Environmental Controls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT Strategy and Policy </t>
-  </si>
-  <si>
-    <t>Network Management and Security</t>
-  </si>
-  <si>
-    <t>Metrics</t>
-  </si>
-  <si>
-    <t>Digital Payment Security Controls(Mobile Payment)</t>
-  </si>
-  <si>
-    <t>Digital Payment Security Controls</t>
-  </si>
-  <si>
-    <t>Inventory Management of Business IT Assets</t>
+    <t>INTERNET BANKING SECURITY
+ CONTROLS</t>
+  </si>
+  <si>
+    <t>Vendor Risk Management</t>
+  </si>
+  <si>
+    <t>Anti-Phishing</t>
   </si>
 </sst>
 </file>
@@ -1030,10 +1034,7 @@
         <v>157</v>
       </c>
       <c r="C2">
-        <v>0.5803248286247253</v>
-      </c>
-      <c r="D2" t="s">
-        <v>161</v>
+        <v>0.8650500178337097</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1044,7 +1045,10 @@
         <v>158</v>
       </c>
       <c r="C3">
-        <v>0.8574562072753906</v>
+        <v>0.6485899686813354</v>
+      </c>
+      <c r="D3" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1055,7 +1059,7 @@
         <v>159</v>
       </c>
       <c r="C4">
-        <v>0.9247996211051941</v>
+        <v>0.9999917149543762</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1066,10 +1070,7 @@
         <v>157</v>
       </c>
       <c r="C5">
-        <v>0.6229012012481689</v>
-      </c>
-      <c r="D5" t="s">
-        <v>166</v>
+        <v>0.9999966025352478</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1080,10 +1081,7 @@
         <v>157</v>
       </c>
       <c r="C6">
-        <v>0.6716668605804443</v>
-      </c>
-      <c r="D6" t="s">
-        <v>172</v>
+        <v>0.9998536109924316</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1094,7 +1092,7 @@
         <v>160</v>
       </c>
       <c r="C7">
-        <v>0.8100273013114929</v>
+        <v>0.9999980330467224</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1102,13 +1100,10 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C8">
-        <v>0.6897293329238892</v>
-      </c>
-      <c r="D8" t="s">
-        <v>183</v>
+        <v>0.9999176859855652</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1116,10 +1111,10 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C9">
-        <v>0.9998621940612793</v>
+        <v>0.9991328716278076</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1127,10 +1122,10 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C10">
-        <v>0.9478148221969604</v>
+        <v>0.9999999403953552</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1138,10 +1133,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C11">
-        <v>0.8725468516349792</v>
+        <v>0.5108258724212646</v>
+      </c>
+      <c r="D11" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1149,13 +1147,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C12">
-        <v>0.6587715148925781</v>
+        <v>0.4966307282447815</v>
       </c>
       <c r="D12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1163,10 +1161,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C13">
-        <v>0.9944120049476624</v>
+        <v>0.4707008898258209</v>
+      </c>
+      <c r="D13" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1174,10 +1175,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C14">
-        <v>0.9706622362136841</v>
+        <v>0.4730821549892426</v>
+      </c>
+      <c r="D14" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1185,10 +1189,10 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C15">
-        <v>0.8468631505966187</v>
+        <v>0.8106363415718079</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1196,10 +1200,10 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C16">
-        <v>0.9999691843986511</v>
+        <v>0.9963210225105286</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1207,10 +1211,10 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C17">
-        <v>0.9896234273910522</v>
+        <v>0.9817414879798889</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1218,10 +1222,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C18">
-        <v>0.9687185287475586</v>
+        <v>0.711452305316925</v>
+      </c>
+      <c r="D18" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1229,13 +1236,10 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C19">
-        <v>0.4791810810565948</v>
-      </c>
-      <c r="D19" t="s">
-        <v>164</v>
+        <v>0.9992054104804993</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1243,13 +1247,10 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C20">
-        <v>0.7584763765335083</v>
-      </c>
-      <c r="D20" t="s">
-        <v>170</v>
+        <v>0.9560477137565613</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1257,10 +1258,10 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C21">
-        <v>0.9362565279006958</v>
+        <v>0.8106440901756287</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1268,13 +1269,10 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="C22">
-        <v>0.5329288840293884</v>
-      </c>
-      <c r="D22" t="s">
-        <v>165</v>
+        <v>0.9999977946281433</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1282,10 +1280,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C23">
-        <v>0.9871996641159058</v>
+        <v>0.6624611616134644</v>
+      </c>
+      <c r="D23" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1293,10 +1294,10 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C24">
-        <v>0.9861684441566467</v>
+        <v>0.9999998211860657</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1304,13 +1305,10 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="C25">
-        <v>0.5088294744491577</v>
-      </c>
-      <c r="D25" t="s">
-        <v>184</v>
+        <v>0.9843375682830811</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1318,10 +1316,13 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="C26">
-        <v>0.985903799533844</v>
+        <v>0.6194658279418945</v>
+      </c>
+      <c r="D26" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1329,13 +1330,10 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="C27">
-        <v>0.696171760559082</v>
-      </c>
-      <c r="D27" t="s">
-        <v>172</v>
+        <v>0.8391256332397461</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1343,10 +1341,10 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C28">
-        <v>0.9991282224655151</v>
+        <v>0.8429456353187561</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1354,10 +1352,10 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C29">
-        <v>0.9999993443489075</v>
+        <v>0.9996986389160156</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1365,10 +1363,10 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C30">
-        <v>0.9862375855445862</v>
+        <v>0.9643871784210205</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1376,10 +1374,10 @@
         <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C31">
-        <v>0.9362565279006958</v>
+        <v>0.8106440901756287</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1387,13 +1385,10 @@
         <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C32">
-        <v>0.758476734161377</v>
-      </c>
-      <c r="D32" t="s">
-        <v>170</v>
+        <v>0.9560479521751404</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1401,13 +1396,10 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="C33">
-        <v>0.6713879108428955</v>
-      </c>
-      <c r="D33" t="s">
-        <v>185</v>
+        <v>0.9997961521148682</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1415,10 +1407,13 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C34">
-        <v>0.9120787382125854</v>
+        <v>0.7249581217765808</v>
+      </c>
+      <c r="D34" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1426,10 +1421,10 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C35">
-        <v>0.4866170585155487</v>
+        <v>0.2546144723892212</v>
       </c>
       <c r="D35" t="s">
         <v>186</v>
@@ -1440,10 +1435,10 @@
         <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C36">
-        <v>0.9896234273910522</v>
+        <v>0.9817414879798889</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1451,10 +1446,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="C37">
-        <v>0.9997464418411255</v>
+        <v>0.9886164665222168</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1462,13 +1457,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C38">
-        <v>0.4666720628738403</v>
+        <v>0.3634660840034485</v>
       </c>
       <c r="D38" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1476,10 +1471,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C39">
-        <v>0.9840673208236694</v>
+        <v>0.9614403247833252</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1487,10 +1482,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="C40">
-        <v>0.9824703931808472</v>
+        <v>0.6029983758926392</v>
+      </c>
+      <c r="D40" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1498,10 +1496,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C41">
-        <v>0.8606067299842834</v>
+        <v>0.7354377508163452</v>
+      </c>
+      <c r="D41" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1509,13 +1510,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="C42">
-        <v>0.3714812695980072</v>
-      </c>
-      <c r="D42" t="s">
-        <v>182</v>
+        <v>0.9995816349983215</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1523,10 +1521,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C43">
-        <v>0.6149329543113708</v>
+        <v>0.2936007082462311</v>
       </c>
       <c r="D43" t="s">
         <v>185</v>
@@ -1537,10 +1535,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C44">
-        <v>0.911519467830658</v>
+        <v>0.9991992115974426</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1548,10 +1546,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C45">
-        <v>0.8628420829772949</v>
+        <v>0.9984164237976074</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1559,10 +1557,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="C46">
-        <v>0.9997591972351074</v>
+        <v>0.9995742440223694</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1570,10 +1568,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="C47">
-        <v>0.8776736259460449</v>
+        <v>0.942889392375946</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1581,10 +1579,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="C48">
-        <v>0.8366320729255676</v>
+        <v>0.5043148398399353</v>
+      </c>
+      <c r="D48" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1592,13 +1593,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="C49">
-        <v>0.5823659896850586</v>
-      </c>
-      <c r="D49" t="s">
-        <v>166</v>
+        <v>0.9899121522903442</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1609,10 +1607,7 @@
         <v>157</v>
       </c>
       <c r="C50">
-        <v>0.4522734582424164</v>
-      </c>
-      <c r="D50" t="s">
-        <v>185</v>
+        <v>0.8693215250968933</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1620,10 +1615,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C51">
-        <v>0.9408423900604248</v>
+        <v>0.9900227189064026</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1631,10 +1626,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C52">
-        <v>0.97287517786026</v>
+        <v>0.9472197294235229</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1642,10 +1637,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C53">
-        <v>0.9999600052833557</v>
+        <v>0.9996703863143921</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1653,10 +1648,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C54">
-        <v>0.8628953099250793</v>
+        <v>0.9993050098419189</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1664,13 +1659,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C55">
-        <v>0.6706184148788452</v>
+        <v>0.5209802985191345</v>
       </c>
       <c r="D55" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1678,13 +1673,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C56">
-        <v>0.688823401927948</v>
-      </c>
-      <c r="D56" t="s">
-        <v>171</v>
+        <v>0.8108912110328674</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1692,10 +1684,13 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C57">
-        <v>0.8606849312782288</v>
+        <v>0.6819602847099304</v>
+      </c>
+      <c r="D57" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1703,10 +1698,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C58">
-        <v>0.9919112324714661</v>
+        <v>0.993499755859375</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1714,13 +1709,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C59">
-        <v>0.7755439877510071</v>
-      </c>
-      <c r="D59" t="s">
-        <v>178</v>
+        <v>0.8797083497047424</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1728,13 +1720,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="C60">
-        <v>0.4971728920936584</v>
-      </c>
-      <c r="D60" t="s">
-        <v>187</v>
+        <v>0.967676043510437</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1742,13 +1731,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="C61">
-        <v>0.4568529427051544</v>
-      </c>
-      <c r="D61" t="s">
-        <v>183</v>
+        <v>0.9839582443237305</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1759,7 +1745,7 @@
         <v>175</v>
       </c>
       <c r="C62">
-        <v>0.9973458647727966</v>
+        <v>0.9595597982406616</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1767,13 +1753,13 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C63">
-        <v>0.4892383813858032</v>
+        <v>0.7287872433662415</v>
       </c>
       <c r="D63" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1781,13 +1767,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C64">
-        <v>0.5325173735618591</v>
+        <v>0.5793125629425049</v>
       </c>
       <c r="D64" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1795,13 +1781,13 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C65">
-        <v>0.378425121307373</v>
+        <v>0.6392939686775208</v>
       </c>
       <c r="D65" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1809,13 +1795,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C66">
-        <v>0.2031905800104141</v>
-      </c>
-      <c r="D66" t="s">
-        <v>172</v>
+        <v>0.9999824166297913</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1823,10 +1806,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C67">
-        <v>0.9931855201721191</v>
+        <v>0.972431480884552</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1834,10 +1817,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="C68">
-        <v>0.9721608757972717</v>
+        <v>0.9871042370796204</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1845,10 +1828,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C69">
-        <v>0.9999960064888</v>
+        <v>0.9646937847137451</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1856,10 +1839,13 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C70">
-        <v>0.9982425570487976</v>
+        <v>0.4041634202003479</v>
+      </c>
+      <c r="D70" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1867,10 +1853,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C71">
-        <v>0.9980023503303528</v>
+        <v>0.9996758699417114</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1878,13 +1864,13 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C72">
-        <v>0.3487241864204407</v>
+        <v>0.6726389527320862</v>
       </c>
       <c r="D72" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1892,13 +1878,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="C73">
-        <v>0.7468725442886353</v>
-      </c>
-      <c r="D73" t="s">
-        <v>158</v>
+        <v>0.9476215839385986</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1906,13 +1889,13 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C74">
-        <v>0.7233596444129944</v>
+        <v>0.7505318522453308</v>
       </c>
       <c r="D74" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1920,13 +1903,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="C75">
-        <v>0.6878369450569153</v>
-      </c>
-      <c r="D75" t="s">
-        <v>163</v>
+        <v>0.9991451501846313</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1934,10 +1914,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C76">
-        <v>0.9999110102653503</v>
+        <v>0.9998414516448975</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1945,13 +1925,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="C77">
-        <v>0.5177441239356995</v>
-      </c>
-      <c r="D77" t="s">
-        <v>170</v>
+        <v>0.9997847080230713</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1959,10 +1936,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C78">
-        <v>0.9995372891426086</v>
+        <v>0.9988299012184143</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1973,10 +1950,7 @@
         <v>157</v>
       </c>
       <c r="C79">
-        <v>0.4299599230289459</v>
-      </c>
-      <c r="D79" t="s">
-        <v>179</v>
+        <v>0.9462848305702209</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1987,7 +1961,7 @@
         <v>167</v>
       </c>
       <c r="C80">
-        <v>0.9672536849975586</v>
+        <v>0.9998295307159424</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1995,10 +1969,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="C81">
-        <v>0.936429500579834</v>
+        <v>0.9243044853210449</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2006,13 +1980,13 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C82">
-        <v>0.7279780507087708</v>
+        <v>0.6972270607948303</v>
       </c>
       <c r="D82" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -2020,10 +1994,13 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C83">
-        <v>0.8924410939216614</v>
+        <v>0.5840380787849426</v>
+      </c>
+      <c r="D83" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -2031,13 +2008,13 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C84">
-        <v>0.6788761019706726</v>
+        <v>0.7000089883804321</v>
       </c>
       <c r="D84" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -2045,10 +2022,13 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="C85">
-        <v>0.8180670738220215</v>
+        <v>0.7093523144721985</v>
+      </c>
+      <c r="D85" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2056,10 +2036,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C86">
-        <v>0.8854007124900818</v>
+        <v>0.9874570369720459</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2067,10 +2047,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="C87">
-        <v>0.9999980330467224</v>
+        <v>0.9022806882858276</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2078,10 +2058,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="C88">
-        <v>0.996501088142395</v>
+        <v>0.9530133008956909</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2089,10 +2069,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C89">
-        <v>0.9999999403953552</v>
+        <v>0.9997580051422119</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2100,13 +2080,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="C90">
-        <v>0.7230919599533081</v>
-      </c>
-      <c r="D90" t="s">
-        <v>185</v>
+        <v>0.999997079372406</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2114,10 +2091,13 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C91">
-        <v>0.8361190557479858</v>
+        <v>0.3239717781543732</v>
+      </c>
+      <c r="D91" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2125,10 +2105,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="C92">
-        <v>0.8767855167388916</v>
+        <v>0.8025994896888733</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2136,10 +2116,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C93">
-        <v>0.9397740960121155</v>
+        <v>0.9936284422874451</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2147,10 +2127,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C94">
-        <v>0.9564576148986816</v>
+        <v>0.9601126909255981</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2158,10 +2138,13 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C95">
-        <v>0.9998540878295898</v>
+        <v>0.7804304957389832</v>
+      </c>
+      <c r="D95" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2169,13 +2152,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C96">
-        <v>0.4847373962402344</v>
-      </c>
-      <c r="D96" t="s">
-        <v>185</v>
+        <v>0.9998459815979004</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2183,10 +2163,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="C97">
-        <v>0.9428815245628357</v>
+        <v>0.9976849555969238</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2197,10 +2177,7 @@
         <v>157</v>
       </c>
       <c r="C98">
-        <v>0.394135057926178</v>
-      </c>
-      <c r="D98" t="s">
-        <v>190</v>
+        <v>0.9671449661254883</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2208,13 +2185,13 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C99">
-        <v>0.796301007270813</v>
+        <v>0.7774090766906738</v>
       </c>
       <c r="D99" t="s">
-        <v>191</v>
+        <v>160</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2222,10 +2199,13 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C100">
-        <v>0.9940020442008972</v>
+        <v>0.7867867946624756</v>
+      </c>
+      <c r="D100" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2233,10 +2213,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="C101">
-        <v>0.8612635135650635</v>
+        <v>0.8523764610290527</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2244,10 +2224,10 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="C102">
-        <v>0.8512932658195496</v>
+        <v>0.9999955296516418</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2255,10 +2235,13 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C103">
-        <v>0.9977708458900452</v>
+        <v>0.6194137334823608</v>
+      </c>
+      <c r="D103" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2266,13 +2249,10 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="C104">
-        <v>0.7737046480178833</v>
-      </c>
-      <c r="D104" t="s">
-        <v>166</v>
+        <v>0.8020535707473755</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -2280,13 +2260,13 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C105">
-        <v>0.3835500180721283</v>
+        <v>0.7555618286132812</v>
       </c>
       <c r="D105" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2294,13 +2274,10 @@
         <v>48</v>
       </c>
       <c r="B106" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="C106">
-        <v>0.5823659896850586</v>
-      </c>
-      <c r="D106" t="s">
-        <v>166</v>
+        <v>0.9899121522903442</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -2311,10 +2288,7 @@
         <v>157</v>
       </c>
       <c r="C107">
-        <v>0.6742856502532959</v>
-      </c>
-      <c r="D107" t="s">
-        <v>175</v>
+        <v>0.9972180128097534</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2322,10 +2296,13 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="C108">
-        <v>0.9095750451087952</v>
+        <v>0.6948152780532837</v>
+      </c>
+      <c r="D108" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2333,10 +2310,10 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C109">
-        <v>0.9985544085502625</v>
+        <v>0.9056593179702759</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2344,13 +2321,10 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C110">
-        <v>0.4203297793865204</v>
-      </c>
-      <c r="D110" t="s">
-        <v>192</v>
+        <v>0.815757691860199</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2358,10 +2332,10 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="C111">
-        <v>0.9998826384544373</v>
+        <v>0.9876804351806641</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2369,10 +2343,10 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="C112">
-        <v>0.8822067975997925</v>
+        <v>0.8013682961463928</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2380,13 +2354,10 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="C113">
-        <v>0.4701441526412964</v>
-      </c>
-      <c r="D113" t="s">
-        <v>181</v>
+        <v>0.8267409801483154</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2394,10 +2365,10 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C114">
-        <v>0.8653886318206787</v>
+        <v>0.9781346917152405</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2405,10 +2376,13 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="C115">
-        <v>0.9994183778762817</v>
+        <v>0.7816182374954224</v>
+      </c>
+      <c r="D115" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2416,13 +2390,10 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C116">
-        <v>0.5802507996559143</v>
-      </c>
-      <c r="D116" t="s">
-        <v>166</v>
+        <v>0.908022403717041</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2430,13 +2401,13 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C117">
-        <v>0.5894866585731506</v>
+        <v>0.5951102375984192</v>
       </c>
       <c r="D117" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2444,13 +2415,10 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C118">
-        <v>0.7032256126403809</v>
-      </c>
-      <c r="D118" t="s">
-        <v>162</v>
+        <v>0.9050993323326111</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2458,13 +2426,13 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C119">
-        <v>0.6384562253952026</v>
+        <v>0.4694755673408508</v>
       </c>
       <c r="D119" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2472,10 +2440,13 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C120">
-        <v>0.8880959153175354</v>
+        <v>0.4474018514156342</v>
+      </c>
+      <c r="D120" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2483,13 +2454,10 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="C121">
-        <v>0.7612026929855347</v>
-      </c>
-      <c r="D121" t="s">
-        <v>172</v>
+        <v>0.9966903328895569</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2497,13 +2465,13 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C122">
-        <v>0.6932358145713806</v>
+        <v>0.6783641576766968</v>
       </c>
       <c r="D122" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2511,10 +2479,10 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C123">
-        <v>0.9405252933502197</v>
+        <v>0.994631826877594</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2522,10 +2490,13 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C124">
-        <v>0.9999989867210388</v>
+        <v>0.4813951253890991</v>
+      </c>
+      <c r="D124" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2536,7 +2507,10 @@
         <v>158</v>
       </c>
       <c r="C125">
-        <v>0.8574562072753906</v>
+        <v>0.6485899686813354</v>
+      </c>
+      <c r="D125" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2547,7 +2521,7 @@
         <v>159</v>
       </c>
       <c r="C126">
-        <v>0.9743465185165405</v>
+        <v>0.9999999403953552</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2555,13 +2529,10 @@
         <v>124</v>
       </c>
       <c r="B127" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="C127">
-        <v>0.3300021588802338</v>
-      </c>
-      <c r="D127" t="s">
-        <v>162</v>
+        <v>0.8132766485214233</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2569,10 +2540,13 @@
         <v>125</v>
       </c>
       <c r="B128" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C128">
-        <v>0.9968034625053406</v>
+        <v>0.7891825437545776</v>
+      </c>
+      <c r="D128" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2580,13 +2554,10 @@
         <v>126</v>
       </c>
       <c r="B129" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="C129">
-        <v>0.4246567189693451</v>
-      </c>
-      <c r="D129" t="s">
-        <v>181</v>
+        <v>0.9999397397041321</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2594,10 +2565,10 @@
         <v>127</v>
       </c>
       <c r="B130" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="C130">
-        <v>0.8883439898490906</v>
+        <v>0.9341633319854736</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2605,13 +2576,10 @@
         <v>128</v>
       </c>
       <c r="B131" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="C131">
-        <v>0.3417912721633911</v>
-      </c>
-      <c r="D131" t="s">
-        <v>172</v>
+        <v>0.9998347759246826</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2619,13 +2587,13 @@
         <v>129</v>
       </c>
       <c r="B132" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C132">
-        <v>0.44663205742836</v>
+        <v>0.5293720960617065</v>
       </c>
       <c r="D132" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2633,10 +2601,10 @@
         <v>130</v>
       </c>
       <c r="B133" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C133">
-        <v>0.9994670152664185</v>
+        <v>0.9845301508903503</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2644,13 +2612,10 @@
         <v>131</v>
       </c>
       <c r="B134" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="C134">
-        <v>0.6934881806373596</v>
-      </c>
-      <c r="D134" t="s">
-        <v>164</v>
+        <v>0.9709152579307556</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2661,10 +2626,7 @@
         <v>157</v>
       </c>
       <c r="C135">
-        <v>0.6962493658065796</v>
-      </c>
-      <c r="D135" t="s">
-        <v>166</v>
+        <v>0.9999999403953552</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2672,10 +2634,10 @@
         <v>133</v>
       </c>
       <c r="B136" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="C136">
-        <v>0.936614453792572</v>
+        <v>0.9991721510887146</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2683,13 +2645,13 @@
         <v>134</v>
       </c>
       <c r="B137" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C137">
-        <v>0.6517713069915771</v>
+        <v>0.7456126809120178</v>
       </c>
       <c r="D137" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2697,10 +2659,10 @@
         <v>135</v>
       </c>
       <c r="B138" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="C138">
-        <v>0.9778202772140503</v>
+        <v>0.9999940991401672</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2708,13 +2670,10 @@
         <v>136</v>
       </c>
       <c r="B139" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="C139">
-        <v>0.691588819026947</v>
-      </c>
-      <c r="D139" t="s">
-        <v>173</v>
+        <v>0.9375523328781128</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2722,13 +2681,10 @@
         <v>137</v>
       </c>
       <c r="B140" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C140">
-        <v>0.6809333562850952</v>
-      </c>
-      <c r="D140" t="s">
-        <v>162</v>
+        <v>0.990467369556427</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -2736,10 +2692,10 @@
         <v>138</v>
       </c>
       <c r="B141" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C141">
-        <v>0.9956642985343933</v>
+        <v>0.9782593846321106</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -2747,10 +2703,10 @@
         <v>139</v>
       </c>
       <c r="B142" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C142">
-        <v>0.8607487678527832</v>
+        <v>0.9996820688247681</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2758,10 +2714,10 @@
         <v>140</v>
       </c>
       <c r="B143" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C143">
-        <v>0.9187852144241333</v>
+        <v>0.9997563362121582</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2769,10 +2725,10 @@
         <v>141</v>
       </c>
       <c r="B144" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C144">
-        <v>0.9342472553253174</v>
+        <v>0.8492854833602905</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2780,10 +2736,10 @@
         <v>142</v>
       </c>
       <c r="B145" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="C145">
-        <v>0.99397873878479</v>
+        <v>0.9996084570884705</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2791,13 +2747,10 @@
         <v>143</v>
       </c>
       <c r="B146" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C146">
-        <v>0.7241778373718262</v>
-      </c>
-      <c r="D146" t="s">
-        <v>171</v>
+        <v>0.9513307213783264</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -2805,10 +2758,10 @@
         <v>144</v>
       </c>
       <c r="B147" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C147">
-        <v>0.999999463558197</v>
+        <v>0.919099748134613</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -2816,10 +2769,10 @@
         <v>145</v>
       </c>
       <c r="B148" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C148">
-        <v>0.9869050979614258</v>
+        <v>0.98480623960495</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -2827,10 +2780,10 @@
         <v>146</v>
       </c>
       <c r="B149" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="C149">
-        <v>0.9838954210281372</v>
+        <v>0.9999956488609314</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -2838,13 +2791,13 @@
         <v>147</v>
       </c>
       <c r="B150" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C150">
-        <v>0.7267008423805237</v>
+        <v>0.5394020080566406</v>
       </c>
       <c r="D150" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -2852,10 +2805,10 @@
         <v>148</v>
       </c>
       <c r="B151" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C151">
-        <v>0.9997828006744385</v>
+        <v>0.9999983906745911</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -2863,13 +2816,10 @@
         <v>149</v>
       </c>
       <c r="B152" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="C152">
-        <v>0.6221325993537903</v>
-      </c>
-      <c r="D152" t="s">
-        <v>167</v>
+        <v>0.9999743103981018</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -2877,10 +2827,10 @@
         <v>150</v>
       </c>
       <c r="B153" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="C153">
-        <v>0.9984245300292969</v>
+        <v>0.8377973437309265</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -2888,13 +2838,13 @@
         <v>151</v>
       </c>
       <c r="B154" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C154">
-        <v>0.6436147093772888</v>
+        <v>0.4653975665569305</v>
       </c>
       <c r="D154" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -2902,13 +2852,10 @@
         <v>152</v>
       </c>
       <c r="B155" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="C155">
-        <v>0.5671029090881348</v>
-      </c>
-      <c r="D155" t="s">
-        <v>166</v>
+        <v>0.9999094009399414</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -2916,10 +2863,10 @@
         <v>153</v>
       </c>
       <c r="B156" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C156">
-        <v>0.9909999966621399</v>
+        <v>0.9334762692451477</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -2927,10 +2874,10 @@
         <v>154</v>
       </c>
       <c r="B157" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="C157">
-        <v>0.9847552180290222</v>
+        <v>0.9888022541999817</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -2938,13 +2885,10 @@
         <v>155</v>
       </c>
       <c r="B158" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C158">
-        <v>0.3935656845569611</v>
-      </c>
-      <c r="D158" t="s">
-        <v>174</v>
+        <v>0.9997510313987732</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -2952,10 +2896,10 @@
         <v>156</v>
       </c>
       <c r="B159" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C159">
-        <v>0.9115321636199951</v>
+        <v>0.8745012879371643</v>
       </c>
     </row>
   </sheetData>

</xml_diff>